<commit_message>
season 4 lesson 097 fix comments
</commit_message>
<xml_diff>
--- a/season-4-lesson-097-Event-Loop-part-002-how-Event-Loop-works-macrotasks-microtasks-requestAnimationFrame/src/Event Loop.xlsx
+++ b/season-4-lesson-097-Event-Loop-part-002-how-Event-Loop-works-macrotasks-microtasks-requestAnimationFrame/src/Event Loop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DevProjects\JSProjects\js-random-lessons\season-4-lesson-097-Event-Loop-part-002-how-Event-Loop-works-macrotasks-microtasks-requestAnimationFrame\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9B9025-4FE6-4F34-8858-2F053ADF5450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF7653F-6764-41E7-BE5D-13B0B43EF22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Call Stack</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>rAF</t>
+  </si>
+  <si>
+    <t>rIC</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +128,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +208,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,39 +499,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:I3"/>
+  <dimension ref="A2:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="9" width="44.7109375" customWidth="1"/>
+    <col min="1" max="8" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>